<commit_message>
Answers to the queries in teh column LN Remarks
</commit_message>
<xml_diff>
--- a/Mobius_Tagmapping_Report_Cases_LawReport.xlsx
+++ b/Mobius_Tagmapping_Report_Cases_LawReport.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Awntika\Project UK_ICS\Mobis\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Awntika\Project UK_ICS\UK-ICS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79AA433F-2920-44BB-8133-ACA158BAC50C}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0EED281-1F30-4627-B128-042E9FB7F604}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="6930" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,12 +20,12 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Element-wise Comparision'!$A$1:$N$853</definedName>
   </definedNames>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="171027"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1385" uniqueCount="844">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1399" uniqueCount="856">
   <si>
     <t>LLRosetta Element</t>
   </si>
@@ -2929,7 +2929,43 @@
     <t>Doesn't matter</t>
   </si>
   <si>
-    <t>Need to check</t>
+    <t>LN Remarks</t>
+  </si>
+  <si>
+    <t>Currently take the value of input. One DB is done will get the values from it</t>
+  </si>
+  <si>
+    <t>This will not be suppressed. If there is no attributes to make the link take it as PC data.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">This coming from the lookup. Currently take the values as it is </t>
+  </si>
+  <si>
+    <t>This will come from the lookup used in metadata for courtcode</t>
+  </si>
+  <si>
+    <t>Need Sample files for this</t>
+  </si>
+  <si>
+    <t>Ther are certain regx used to manage dates. Will share that</t>
+  </si>
+  <si>
+    <t>If pcdata is present in any *:date element the &lt;date day='' month='' year='' &gt; will be created with the respective attribute values.</t>
+  </si>
+  <si>
+    <t>Need samples</t>
+  </si>
+  <si>
+    <t>Need Samples</t>
+  </si>
+  <si>
+    <t>searchtype attribute value can be taken as it is. Normcite will be created by concatenated value of ci:sesslawnum and ci:hierpinpoint and ci:standardname. If hierpinpoint is not available just take the values of ci:standardname and ci:hierpinpoint. Can discuss this if any queries</t>
+  </si>
+  <si>
+    <t>Do not suppress glp:note even if its done in LA.Tak it as it is.</t>
+  </si>
+  <si>
+    <t>In discussion</t>
   </si>
 </sst>
 </file>
@@ -3099,7 +3135,7 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="47">
+  <cellXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -3199,11 +3235,9 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -3212,14 +3246,23 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -5124,7 +5167,7 @@
       <c r="J67" s="17"/>
       <c r="K67" s="17"/>
       <c r="L67" s="17"/>
-      <c r="M67" s="39" t="s">
+      <c r="M67" s="44" t="s">
         <v>115</v>
       </c>
       <c r="N67" s="17"/>
@@ -5144,7 +5187,7 @@
       <c r="J68" s="17"/>
       <c r="K68" s="17"/>
       <c r="L68" s="17"/>
-      <c r="M68" s="39"/>
+      <c r="M68" s="44"/>
       <c r="N68" s="17"/>
     </row>
     <row r="69" spans="1:14">
@@ -5202,7 +5245,7 @@
       <c r="J71" s="17"/>
       <c r="K71" s="17"/>
       <c r="L71" s="17"/>
-      <c r="M71" s="40" t="s">
+      <c r="M71" s="43" t="s">
         <v>121</v>
       </c>
       <c r="N71" s="17"/>
@@ -5222,7 +5265,7 @@
       <c r="J72" s="17"/>
       <c r="K72" s="17"/>
       <c r="L72" s="17"/>
-      <c r="M72" s="40"/>
+      <c r="M72" s="43"/>
       <c r="N72" s="17"/>
     </row>
     <row r="73" spans="1:14">
@@ -5240,7 +5283,7 @@
       <c r="J73" s="17"/>
       <c r="K73" s="17"/>
       <c r="L73" s="17"/>
-      <c r="M73" s="40"/>
+      <c r="M73" s="43"/>
       <c r="N73" s="17"/>
     </row>
     <row r="74" spans="1:14">
@@ -5258,7 +5301,7 @@
       <c r="J74" s="17"/>
       <c r="K74" s="17"/>
       <c r="L74" s="17"/>
-      <c r="M74" s="40"/>
+      <c r="M74" s="43"/>
       <c r="N74" s="17"/>
     </row>
     <row r="75" spans="1:14">
@@ -5478,7 +5521,7 @@
       <c r="J85" s="17"/>
       <c r="K85" s="17"/>
       <c r="L85" s="17"/>
-      <c r="M85" s="40" t="s">
+      <c r="M85" s="43" t="s">
         <v>140</v>
       </c>
       <c r="N85" s="17"/>
@@ -5498,7 +5541,7 @@
       <c r="J86" s="17"/>
       <c r="K86" s="17"/>
       <c r="L86" s="17"/>
-      <c r="M86" s="40"/>
+      <c r="M86" s="43"/>
       <c r="N86" s="17"/>
     </row>
     <row r="87" spans="1:14">
@@ -5556,7 +5599,7 @@
       <c r="J89" s="17"/>
       <c r="K89" s="17"/>
       <c r="L89" s="17"/>
-      <c r="M89" s="40" t="s">
+      <c r="M89" s="43" t="s">
         <v>146</v>
       </c>
       <c r="N89" s="17"/>
@@ -5576,7 +5619,7 @@
       <c r="J90" s="17"/>
       <c r="K90" s="17"/>
       <c r="L90" s="17"/>
-      <c r="M90" s="40"/>
+      <c r="M90" s="43"/>
       <c r="N90" s="17"/>
     </row>
     <row r="91" spans="1:14">
@@ -5594,7 +5637,7 @@
       <c r="J91" s="17"/>
       <c r="K91" s="17"/>
       <c r="L91" s="17"/>
-      <c r="M91" s="40"/>
+      <c r="M91" s="43"/>
       <c r="N91" s="17"/>
     </row>
     <row r="92" spans="1:14">
@@ -5612,7 +5655,7 @@
       <c r="J92" s="17"/>
       <c r="K92" s="17"/>
       <c r="L92" s="17"/>
-      <c r="M92" s="40"/>
+      <c r="M92" s="43"/>
       <c r="N92" s="17"/>
     </row>
     <row r="93" spans="1:14">
@@ -6484,7 +6527,7 @@
       <c r="J136" s="17"/>
       <c r="K136" s="17"/>
       <c r="L136" s="17"/>
-      <c r="M136" s="40"/>
+      <c r="M136" s="43"/>
       <c r="N136" s="17"/>
     </row>
     <row r="137" spans="1:14">
@@ -7192,7 +7235,7 @@
       <c r="J172" s="17"/>
       <c r="K172" s="17"/>
       <c r="L172" s="17"/>
-      <c r="M172" s="40"/>
+      <c r="M172" s="43"/>
       <c r="N172" s="17"/>
     </row>
     <row r="173" spans="1:14">
@@ -11344,7 +11387,7 @@
       <c r="J386" s="17"/>
       <c r="K386" s="17"/>
       <c r="L386" s="17"/>
-      <c r="M386" s="40"/>
+      <c r="M386" s="43"/>
       <c r="N386" s="17"/>
     </row>
     <row r="387" spans="1:14">
@@ -12182,7 +12225,7 @@
       <c r="J428" s="17"/>
       <c r="K428" s="17"/>
       <c r="L428" s="17"/>
-      <c r="M428" s="40"/>
+      <c r="M428" s="43"/>
       <c r="N428" s="17"/>
     </row>
     <row r="429" spans="1:14">
@@ -12714,7 +12757,7 @@
       <c r="J451" s="17"/>
       <c r="K451" s="17"/>
       <c r="L451" s="17"/>
-      <c r="M451" s="40"/>
+      <c r="M451" s="43"/>
       <c r="N451" s="17"/>
     </row>
     <row r="452" spans="1:14" ht="120">
@@ -12812,7 +12855,7 @@
       <c r="J456" s="17"/>
       <c r="K456" s="17"/>
       <c r="L456" s="17"/>
-      <c r="M456" s="40"/>
+      <c r="M456" s="43"/>
       <c r="N456" s="17"/>
     </row>
     <row r="457" spans="1:14">
@@ -12870,7 +12913,7 @@
       <c r="J459" s="17"/>
       <c r="K459" s="17"/>
       <c r="L459" s="17"/>
-      <c r="M459" s="40"/>
+      <c r="M459" s="43"/>
       <c r="N459" s="17"/>
     </row>
     <row r="460" spans="1:14" ht="75">
@@ -16461,6 +16504,36 @@
   </sheetData>
   <autoFilter ref="A1:N853" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <mergeCells count="38">
+    <mergeCell ref="M67:M68"/>
+    <mergeCell ref="M71:M74"/>
+    <mergeCell ref="M85:M86"/>
+    <mergeCell ref="M89:M92"/>
+    <mergeCell ref="M103:M104"/>
+    <mergeCell ref="M107:M110"/>
+    <mergeCell ref="M124:M127"/>
+    <mergeCell ref="M135:M136"/>
+    <mergeCell ref="M139:M142"/>
+    <mergeCell ref="M153:M154"/>
+    <mergeCell ref="M157:M160"/>
+    <mergeCell ref="M171:M172"/>
+    <mergeCell ref="M175:M178"/>
+    <mergeCell ref="M192:M193"/>
+    <mergeCell ref="M197:M200"/>
+    <mergeCell ref="M375:M376"/>
+    <mergeCell ref="M382:M384"/>
+    <mergeCell ref="M385:M386"/>
+    <mergeCell ref="M396:M397"/>
+    <mergeCell ref="M404:M406"/>
+    <mergeCell ref="M407:M408"/>
+    <mergeCell ref="M419:M420"/>
+    <mergeCell ref="M421:M422"/>
+    <mergeCell ref="M424:M426"/>
+    <mergeCell ref="M427:M428"/>
+    <mergeCell ref="M450:M451"/>
+    <mergeCell ref="M455:M456"/>
+    <mergeCell ref="M458:M459"/>
+    <mergeCell ref="M462:M464"/>
+    <mergeCell ref="M465:M466"/>
     <mergeCell ref="M486:M488"/>
     <mergeCell ref="M489:M490"/>
     <mergeCell ref="N492:N498"/>
@@ -16469,36 +16542,6 @@
     <mergeCell ref="M477:M478"/>
     <mergeCell ref="M480:M482"/>
     <mergeCell ref="M483:M484"/>
-    <mergeCell ref="M450:M451"/>
-    <mergeCell ref="M455:M456"/>
-    <mergeCell ref="M458:M459"/>
-    <mergeCell ref="M462:M464"/>
-    <mergeCell ref="M465:M466"/>
-    <mergeCell ref="M407:M408"/>
-    <mergeCell ref="M419:M420"/>
-    <mergeCell ref="M421:M422"/>
-    <mergeCell ref="M424:M426"/>
-    <mergeCell ref="M427:M428"/>
-    <mergeCell ref="M375:M376"/>
-    <mergeCell ref="M382:M384"/>
-    <mergeCell ref="M385:M386"/>
-    <mergeCell ref="M396:M397"/>
-    <mergeCell ref="M404:M406"/>
-    <mergeCell ref="M157:M160"/>
-    <mergeCell ref="M171:M172"/>
-    <mergeCell ref="M175:M178"/>
-    <mergeCell ref="M192:M193"/>
-    <mergeCell ref="M197:M200"/>
-    <mergeCell ref="M107:M110"/>
-    <mergeCell ref="M124:M127"/>
-    <mergeCell ref="M135:M136"/>
-    <mergeCell ref="M139:M142"/>
-    <mergeCell ref="M153:M154"/>
-    <mergeCell ref="M67:M68"/>
-    <mergeCell ref="M71:M74"/>
-    <mergeCell ref="M85:M86"/>
-    <mergeCell ref="M89:M92"/>
-    <mergeCell ref="M103:M104"/>
   </mergeCells>
   <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait"/>
@@ -16509,8 +16552,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A2:F64"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A35" workbookViewId="0">
-      <selection activeCell="A38" sqref="A38"/>
+    <sheetView tabSelected="1" topLeftCell="C49" workbookViewId="0">
+      <selection activeCell="G49" sqref="G49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -16520,37 +16563,38 @@
     <col min="3" max="3" width="57.7109375" style="9" customWidth="1"/>
     <col min="4" max="4" width="34.85546875" style="5" customWidth="1"/>
     <col min="5" max="5" width="24.5703125" style="9" customWidth="1"/>
-    <col min="6" max="16384" width="9" style="5"/>
+    <col min="6" max="6" width="29.140625" style="5" customWidth="1"/>
+    <col min="7" max="16384" width="9" style="5"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:5">
-      <c r="A2" s="44" t="s">
+    <row r="2" spans="1:6">
+      <c r="A2" s="46" t="s">
         <v>780</v>
       </c>
-      <c r="B2" s="44"/>
-      <c r="C2" s="44"/>
-    </row>
-    <row r="3" spans="1:5" ht="15" customHeight="1">
-      <c r="A3" s="44"/>
-      <c r="B3" s="44"/>
-      <c r="C3" s="44"/>
-    </row>
-    <row r="4" spans="1:5">
-      <c r="A4" s="44"/>
-      <c r="B4" s="44"/>
-      <c r="C4" s="44"/>
-    </row>
-    <row r="5" spans="1:5">
-      <c r="A5" s="44"/>
-      <c r="B5" s="44"/>
-      <c r="C5" s="44"/>
-    </row>
-    <row r="6" spans="1:5">
-      <c r="A6" s="44"/>
-      <c r="B6" s="44"/>
-      <c r="C6" s="44"/>
-    </row>
-    <row r="8" spans="1:5">
+      <c r="B2" s="46"/>
+      <c r="C2" s="46"/>
+    </row>
+    <row r="3" spans="1:6" ht="15" customHeight="1">
+      <c r="A3" s="46"/>
+      <c r="B3" s="46"/>
+      <c r="C3" s="46"/>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="A4" s="46"/>
+      <c r="B4" s="46"/>
+      <c r="C4" s="46"/>
+    </row>
+    <row r="5" spans="1:6">
+      <c r="A5" s="46"/>
+      <c r="B5" s="46"/>
+      <c r="C5" s="46"/>
+    </row>
+    <row r="6" spans="1:6">
+      <c r="A6" s="46"/>
+      <c r="B6" s="46"/>
+      <c r="C6" s="46"/>
+    </row>
+    <row r="8" spans="1:6" ht="30">
       <c r="A8" s="10" t="s">
         <v>781</v>
       </c>
@@ -16566,8 +16610,11 @@
       <c r="E8" s="11" t="s">
         <v>785</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" s="6" customFormat="1" ht="15" customHeight="1">
+      <c r="F8" s="47" t="s">
+        <v>843</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" s="6" customFormat="1" ht="15" customHeight="1">
       <c r="A9" s="12" t="s">
         <v>10</v>
       </c>
@@ -16578,7 +16625,7 @@
       <c r="D9" s="14"/>
       <c r="E9" s="13"/>
     </row>
-    <row r="10" spans="1:5" s="6" customFormat="1" ht="15" customHeight="1">
+    <row r="10" spans="1:6" s="6" customFormat="1" ht="15" customHeight="1">
       <c r="A10" s="12" t="s">
         <v>15</v>
       </c>
@@ -16589,7 +16636,7 @@
       <c r="D10" s="14"/>
       <c r="E10" s="13"/>
     </row>
-    <row r="11" spans="1:5" s="6" customFormat="1" ht="84.95" customHeight="1">
+    <row r="11" spans="1:6" s="6" customFormat="1" ht="84.95" customHeight="1">
       <c r="A11" s="15" t="s">
         <v>21</v>
       </c>
@@ -16601,8 +16648,11 @@
       </c>
       <c r="D11" s="14"/>
       <c r="E11" s="13"/>
-    </row>
-    <row r="12" spans="1:5" s="6" customFormat="1" ht="15" customHeight="1">
+      <c r="F11" s="6" t="s">
+        <v>844</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" s="6" customFormat="1" ht="15" customHeight="1">
       <c r="A12" s="17" t="s">
         <v>35</v>
       </c>
@@ -16613,7 +16663,7 @@
       <c r="D12" s="14"/>
       <c r="E12" s="13"/>
     </row>
-    <row r="13" spans="1:5" s="6" customFormat="1" ht="15" customHeight="1">
+    <row r="13" spans="1:6" s="6" customFormat="1" ht="15" customHeight="1">
       <c r="A13" s="12" t="s">
         <v>38</v>
       </c>
@@ -16623,8 +16673,11 @@
       <c r="C13" s="13"/>
       <c r="D13" s="14"/>
       <c r="E13" s="13"/>
-    </row>
-    <row r="14" spans="1:5" s="6" customFormat="1" ht="105.95" customHeight="1">
+      <c r="F13" s="6" t="s">
+        <v>845</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" s="6" customFormat="1" ht="105.95" customHeight="1">
       <c r="A14" s="12" t="s">
         <v>65</v>
       </c>
@@ -16640,8 +16693,11 @@
       <c r="E14" s="13" t="s">
         <v>792</v>
       </c>
-    </row>
-    <row r="15" spans="1:5" s="6" customFormat="1" ht="15" customHeight="1">
+      <c r="F14" s="40" t="s">
+        <v>846</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" s="6" customFormat="1" ht="15" customHeight="1">
       <c r="A15" s="12" t="s">
         <v>793</v>
       </c>
@@ -16653,8 +16709,11 @@
       </c>
       <c r="D15" s="14"/>
       <c r="E15" s="13"/>
-    </row>
-    <row r="16" spans="1:5" s="6" customFormat="1" ht="15" customHeight="1">
+      <c r="F15" s="48" t="s">
+        <v>848</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" s="6" customFormat="1" ht="15" customHeight="1">
       <c r="A16" s="12" t="s">
         <v>317</v>
       </c>
@@ -16677,6 +16736,9 @@
       <c r="C17" s="13"/>
       <c r="D17" s="14"/>
       <c r="E17" s="13"/>
+      <c r="F17" s="6" t="s">
+        <v>847</v>
+      </c>
     </row>
     <row r="18" spans="1:6" s="6" customFormat="1" ht="15" customHeight="1">
       <c r="A18" s="12" t="s">
@@ -16699,8 +16761,11 @@
       <c r="C19" s="13"/>
       <c r="D19" s="14"/>
       <c r="E19" s="13"/>
-    </row>
-    <row r="20" spans="1:6" s="6" customFormat="1" ht="66" customHeight="1">
+      <c r="F19" s="48" t="s">
+        <v>849</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" s="6" customFormat="1" ht="75">
       <c r="A20" s="12"/>
       <c r="B20" s="12" t="s">
         <v>499</v>
@@ -16710,8 +16775,11 @@
       </c>
       <c r="D20" s="14"/>
       <c r="E20" s="13"/>
-    </row>
-    <row r="21" spans="1:6" s="6" customFormat="1" ht="48" customHeight="1">
+      <c r="F20" s="49" t="s">
+        <v>850</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" s="6" customFormat="1" ht="60">
       <c r="A21" s="12" t="s">
         <v>706</v>
       </c>
@@ -16723,6 +16791,9 @@
       </c>
       <c r="D21" s="14"/>
       <c r="E21" s="13"/>
+      <c r="F21" s="48" t="s">
+        <v>851</v>
+      </c>
     </row>
     <row r="22" spans="1:6" s="6" customFormat="1" ht="15" customHeight="1">
       <c r="A22" s="12" t="s">
@@ -16745,6 +16816,9 @@
       </c>
       <c r="D23" s="14"/>
       <c r="E23" s="13"/>
+      <c r="F23" s="48" t="s">
+        <v>852</v>
+      </c>
     </row>
     <row r="24" spans="1:6" s="6" customFormat="1" ht="24" customHeight="1">
       <c r="A24" s="12" t="s">
@@ -16757,7 +16831,7 @@
       <c r="D24" s="14"/>
       <c r="E24" s="13"/>
     </row>
-    <row r="25" spans="1:6" s="6" customFormat="1" ht="126" customHeight="1">
+    <row r="25" spans="1:6" s="6" customFormat="1" ht="165">
       <c r="A25" s="13" t="s">
         <v>79</v>
       </c>
@@ -16769,8 +16843,8 @@
       </c>
       <c r="D25" s="14"/>
       <c r="E25" s="13"/>
-      <c r="F25" s="46" t="s">
-        <v>843</v>
+      <c r="F25" s="40" t="s">
+        <v>853</v>
       </c>
     </row>
     <row r="26" spans="1:6" s="6" customFormat="1" ht="15" customHeight="1">
@@ -16843,6 +16917,9 @@
       <c r="C31" s="13"/>
       <c r="D31" s="14"/>
       <c r="E31" s="13"/>
+      <c r="F31" s="6" t="s">
+        <v>854</v>
+      </c>
     </row>
     <row r="32" spans="1:6" s="6" customFormat="1" ht="15" customHeight="1">
       <c r="A32" s="12" t="s">
@@ -16880,6 +16957,9 @@
       <c r="E34" s="13" t="s">
         <v>805</v>
       </c>
+      <c r="F34" s="7" t="s">
+        <v>855</v>
+      </c>
     </row>
     <row r="35" spans="1:6" s="6" customFormat="1" ht="90">
       <c r="A35" s="12" t="s">
@@ -16895,6 +16975,9 @@
       <c r="E35" s="13" t="s">
         <v>808</v>
       </c>
+      <c r="F35" s="7" t="s">
+        <v>855</v>
+      </c>
     </row>
     <row r="36" spans="1:6" s="6" customFormat="1" ht="75">
       <c r="A36" s="12" t="s">
@@ -16909,6 +16992,9 @@
       <c r="D36" s="14"/>
       <c r="E36" s="13" t="s">
         <v>810</v>
+      </c>
+      <c r="F36" s="7" t="s">
+        <v>855</v>
       </c>
     </row>
     <row r="37" spans="1:6" s="6" customFormat="1" ht="90">
@@ -17000,7 +17086,7 @@
       </c>
     </row>
     <row r="43" spans="1:6" s="6" customFormat="1">
-      <c r="A43" s="43" t="s">
+      <c r="A43" s="45" t="s">
         <v>649</v>
       </c>
       <c r="B43" s="12" t="s">
@@ -17015,7 +17101,7 @@
       </c>
     </row>
     <row r="44" spans="1:6" s="6" customFormat="1">
-      <c r="A44" s="43"/>
+      <c r="A44" s="45"/>
       <c r="B44" s="12" t="s">
         <v>667</v>
       </c>
@@ -17078,7 +17164,7 @@
       <c r="E48" s="22" t="s">
         <v>824</v>
       </c>
-      <c r="F48" s="45" t="s">
+      <c r="F48" s="39" t="s">
         <v>841</v>
       </c>
     </row>

</xml_diff>